<commit_message>
Started working on Mage skill tree
</commit_message>
<xml_diff>
--- a/Untitled-RPG/Assets/Excel/Skills.xlsx
+++ b/Untitled-RPG/Assets/Excel/Skills.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Untitled-RPG\Untitled-RPG\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233D93BA-82E7-48EF-B24C-0711636A5C9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552A1A53-6CBF-45A0-A7AC-07D547771231}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9315256A-FBE0-4846-A7B0-BE8037A06B15}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>Knight</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Mage</t>
+  </si>
+  <si>
+    <t>Fireball</t>
+  </si>
+  <si>
+    <t>Casts fireball at a target dealing instant damage, plus setting the target on  fire dealing reoccurring damage for 5 seconds. Instant</t>
   </si>
 </sst>
 </file>
@@ -149,7 +158,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +174,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0DCB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -205,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -227,12 +242,23 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0DCB"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -541,17 +567,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8A2020-1350-429C-A7A8-844477B7E611}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="117.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
@@ -753,11 +779,136 @@
         <v>30</v>
       </c>
     </row>
+    <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1000</v>
+      </c>
+      <c r="F13" s="8">
+        <v>100</v>
+      </c>
+      <c r="G13" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>8</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>10</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>11</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>12</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>13</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -765,7 +916,7 @@
           <x14:formula1>
             <xm:f>Variables!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D9</xm:sqref>
+          <xm:sqref>D3:D9 D13:D19</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Started working on levitation
</commit_message>
<xml_diff>
--- a/Untitled-RPG/Assets/Excel/Skills.xlsx
+++ b/Untitled-RPG/Assets/Excel/Skills.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Untitled-RPG\Untitled-RPG\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552A1A53-6CBF-45A0-A7AC-07D547771231}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C91097-7B05-4434-B753-98F2618E4890}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9315256A-FBE0-4846-A7B0-BE8037A06B15}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Knight</t>
   </si>
@@ -127,6 +127,24 @@
   </si>
   <si>
     <t>Casts fireball at a target dealing instant damage, plus setting the target on  fire dealing reoccurring damage for 5 seconds. Instant</t>
+  </si>
+  <si>
+    <t>Firewall</t>
+  </si>
+  <si>
+    <t>Hailstone</t>
+  </si>
+  <si>
+    <t>Power-sphere</t>
+  </si>
+  <si>
+    <t>Lightning</t>
+  </si>
+  <si>
+    <t>Levitation</t>
+  </si>
+  <si>
+    <t>Armageddon</t>
   </si>
 </sst>
 </file>
@@ -570,13 +588,13 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="117.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -840,7 +858,9 @@
       <c r="A14" s="3">
         <v>8</v>
       </c>
-      <c r="B14" s="7"/>
+      <c r="B14" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -851,7 +871,9 @@
       <c r="A15" s="3">
         <v>9</v>
       </c>
-      <c r="B15" s="7"/>
+      <c r="B15" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -862,7 +884,9 @@
       <c r="A16" s="3">
         <v>10</v>
       </c>
-      <c r="B16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -873,7 +897,9 @@
       <c r="A17" s="3">
         <v>11</v>
       </c>
-      <c r="B17" s="7"/>
+      <c r="B17" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -884,7 +910,9 @@
       <c r="A18" s="3">
         <v>12</v>
       </c>
-      <c r="B18" s="7"/>
+      <c r="B18" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -895,7 +923,9 @@
       <c r="A19" s="3">
         <v>13</v>
       </c>
-      <c r="B19" s="7"/>
+      <c r="B19" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>

</xml_diff>